<commit_message>
Add discount handling in order summary update; connect discount input to UI
</commit_message>
<xml_diff>
--- a/Backup/Orders.xlsx
+++ b/Backup/Orders.xlsx
@@ -972,7 +972,7 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>31.89830508474576</v>
+        <v>1761.823668009425</v>
       </c>
       <c r="F20" t="n">
         <v>0</v>
@@ -1301,7 +1301,11 @@
       <c r="F32" t="n">
         <v>0</v>
       </c>
-      <c r="G32" t="inlineStr"/>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>281TOT</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -1324,7 +1328,11 @@
       <c r="F33" t="n">
         <v>0</v>
       </c>
-      <c r="G33" t="inlineStr"/>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>108</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="n">

</xml_diff>